<commit_message>
Story Time (Full Version Update 2)
Test case updated.
</commit_message>
<xml_diff>
--- a/test_cases/Features Test Case Story Time.xlsx
+++ b/test_cases/Features Test Case Story Time.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -163,6 +163,9 @@
     <t xml:space="preserve">Plays the introduction</t>
   </si>
   <si>
+    <t xml:space="preserve">Played the introduction</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pass</t>
   </si>
   <si>
@@ -255,8 +258,6 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Command “next”
-Command “stop”
-Command “replay”
 </t>
     </r>
     <r>
@@ -289,25 +290,35 @@
     <t xml:space="preserve">The robot waits</t>
   </si>
   <si>
+    <t xml:space="preserve">The robot waited</t>
+  </si>
+  <si>
     <t xml:space="preserve">Robot hears “next” from the person</t>
   </si>
   <si>
     <t xml:space="preserve">The robot understands then speaks the next page.</t>
   </si>
   <si>
+    <t xml:space="preserve">The robot understood then spoke the next page.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Robot hears “next” from the person but there are no more pages for the robot to read.</t>
   </si>
   <si>
     <t xml:space="preserve">The robot says “The End” then links to the stopped command dialogue.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+    <t xml:space="preserve">The robot said “The End” then linked to the stopped command dialogue.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Given: </t>
     </r>
@@ -317,6 +328,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Robot has finished reading a page
 </t>
@@ -328,6 +340,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 When: </t>
@@ -338,6 +351,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">It has given a response “stop” 
 </t>
@@ -349,6 +363,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 Then: </t>
@@ -359,6 +374,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">It will say “Thank you, time to stop reading.” Then end the program
 </t>
@@ -381,9 +397,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Command “next”
-Command “stop”
-Command “replay”
+      <t xml:space="preserve">Command “stop”
 </t>
     </r>
     <r>
@@ -412,6 +426,9 @@
   </si>
   <si>
     <t xml:space="preserve">The robot will say “Thank you, time to stop reading.” Then end the program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The robot said “Thank you, time to stop reading.” Then ended the program</t>
   </si>
   <si>
     <r>
@@ -503,7 +520,6 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Command “yes”
-Command “no”
 </t>
     </r>
     <r>
@@ -534,6 +550,9 @@
   </si>
   <si>
     <t xml:space="preserve">The robot understands then gives instructions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The robot understood then gave the instructions.</t>
   </si>
   <si>
     <r>
@@ -624,8 +643,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Command “yes”
-Command “no”
+      <t xml:space="preserve">Command “no”
 </t>
     </r>
     <r>
@@ -658,13 +676,17 @@
     <t xml:space="preserve">The robot understands then ends the program.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+    <t xml:space="preserve">The robot understood then ended the program.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Given: </t>
     </r>
@@ -674,6 +696,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Robot has finished reading a page
 </t>
@@ -685,6 +708,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 When: </t>
@@ -695,6 +719,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">It has given a response “replay” 
 </t>
@@ -706,6 +731,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 Then: </t>
@@ -716,6 +742,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">It will replay the page it just read with animations if necessary.
 </t>
@@ -727,6 +754,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Prerequisite: 
 </t>
@@ -737,19 +765,19 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Command “next”
-Command “stop”
-Command “replay”
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Command “replay”
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Test Data:
 </t>
@@ -760,6 +788,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Prompt response “replay”</t>
     </r>
@@ -769,6 +798,9 @@
   </si>
   <si>
     <t xml:space="preserve">The robot will replay the page it just read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The robot replayed the page it just read</t>
   </si>
   <si>
     <r>
@@ -1086,20 +1118,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1120,8 +1152,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF72BF44"/>
       </patternFill>
     </fill>
   </fills>
@@ -1166,7 +1204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1227,7 +1265,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1235,11 +1273,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1301,7 +1335,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1322,8 +1356,8 @@
   </sheetPr>
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1401,11 +1435,11 @@
       <c r="G3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>12</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J3" s="16"/>
     </row>
@@ -1455,22 +1489,22 @@
         <v>1.02</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J7" s="16"/>
     </row>
@@ -1482,16 +1516,16 @@
         <v>2</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J8" s="16"/>
     </row>
@@ -1502,17 +1536,17 @@
       <c r="E9" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>18</v>
+      <c r="F9" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J9" s="16"/>
     </row>
@@ -1534,23 +1568,23 @@
       <c r="C11" s="12" t="n">
         <v>1.03</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>20</v>
+      <c r="D11" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J11" s="16"/>
     </row>
@@ -1562,16 +1596,16 @@
         <v>2</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J12" s="16"/>
     </row>
@@ -1607,22 +1641,22 @@
         <v>1.04</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E15" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J15" s="16"/>
     </row>
@@ -1634,16 +1668,16 @@
         <v>2</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J16" s="16"/>
     </row>
@@ -1654,9 +1688,9 @@
       <c r="E17" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="16"/>
     </row>
@@ -1679,22 +1713,22 @@
         <v>1.05</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E19" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J19" s="16"/>
     </row>
@@ -1706,16 +1740,16 @@
         <v>2</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J20" s="16"/>
     </row>
@@ -1726,9 +1760,9 @@
       <c r="E21" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="16"/>
     </row>
@@ -1750,23 +1784,23 @@
       <c r="C23" s="12" t="n">
         <v>1.06</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>29</v>
+      <c r="D23" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="E23" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J23" s="16"/>
     </row>
@@ -1778,16 +1812,16 @@
         <v>2</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>12</v>
+        <v>37</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="J24" s="16"/>
     </row>
@@ -1920,7 +1954,7 @@
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>1</v>
@@ -1974,7 +2008,7 @@
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E7" s="11" t="n">
         <v>1</v>
@@ -2028,7 +2062,7 @@
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="13" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E11" s="11" t="n">
         <v>1</v>
@@ -2128,10 +2162,10 @@
     <row r="1" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="5"/>
       <c r="C1" s="8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>3</v>
@@ -2151,28 +2185,28 @@
     </row>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="11" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>1.01</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E2" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>12</v>
+        <v>47</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,16 +2217,16 @@
         <v>2</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2203,16 +2237,16 @@
         <v>3</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>12</v>
+        <v>53</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="153.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2223,16 +2257,16 @@
         <v>4</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>